<commit_message>
Add GitHub Pages deployment with static HTML landing page
</commit_message>
<xml_diff>
--- a/output/extracted_cards.xlsx
+++ b/output/extracted_cards.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Business Cards" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Business Cards'!$A$1:$H$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Business Cards'!$A$1:$H$7</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,33 +512,33 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>Olivia Wilson</t>
+          <t>Nehaal Fakih</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>Real Estate Agent</t>
+          <t>SPRINGBOARD</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr"/>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>+123-456-7890, +123-456-7890</t>
+          <t>+91-9004488330</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>hello@reallygreatsite.com</t>
+          <t>nehaal@91springboard.com</t>
         </is>
       </c>
       <c r="G2" s="3" t="inlineStr">
         <is>
-          <t>WWWreallygreatsite.com</t>
+          <t>91springboard.com</t>
         </is>
       </c>
       <c r="H2" s="3" t="inlineStr">
         <is>
-          <t>123 Anywhere St;_, City, ST 12345</t>
+          <t>Plot No. D-5 Road No. 20, Marol MIDC, Andheri East</t>
         </is>
       </c>
     </row>
@@ -548,34 +548,150 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>FineFX</t>
+          <t>Tel</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>Sandra</t>
-        </is>
-      </c>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>Art Director</t>
-        </is>
-      </c>
+          <t>SRIMATHA</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr"/>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>206-353-2846</t>
-        </is>
-      </c>
-      <c r="F3" s="3" t="inlineStr"/>
-      <c r="G3" s="3" t="inlineStr"/>
-      <c r="H3" s="3" t="inlineStr">
-        <is>
-          <t>20098 Piney Point Rd,Callaway;</t>
-        </is>
-      </c>
+          <t>(08814)224530, 224796 (0), 94401 80153</t>
+        </is>
+      </c>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>Ivrcocoanutmerchants@gmail.com</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>M.Narayana</t>
+        </is>
+      </c>
+      <c r="H3" s="3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>CA</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>Near Hotel</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr"/>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>91 9730704929, 91 9421833600</t>
+        </is>
+      </c>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>capushkarsolanki@gmail.com</t>
+        </is>
+      </c>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
+          <t>B.Com</t>
+        </is>
+      </c>
+      <c r="H4" s="3" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>Bhavesh</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>Shreenath</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>Sales Corporation</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>93253 13803, 99675 53803</t>
+        </is>
+      </c>
+      <c r="F5" s="3" t="inlineStr"/>
+      <c r="G5" s="3" t="inlineStr"/>
+      <c r="H5" s="3" t="inlineStr">
+        <is>
+          <t>Off Link Road, Mahavir Nagar;</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>Plywood</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>Laminates</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="inlineStr"/>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>9370762286, 9373962286, 0253-2462286</t>
+        </is>
+      </c>
+      <c r="F6" s="3" t="inlineStr"/>
+      <c r="G6" s="3" t="inlineStr"/>
+      <c r="H6" s="3" t="inlineStr">
+        <is>
+          <t>Nashik Road</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>MANAVTA</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>Gram</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="inlineStr"/>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>(0) 6501982, 4618756, 4618738</t>
+        </is>
+      </c>
+      <c r="F7" s="3" t="inlineStr"/>
+      <c r="G7" s="3" t="inlineStr"/>
+      <c r="H7" s="3" t="inlineStr"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H3"/>
+  <autoFilter ref="A1:H7"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>